<commit_message>
Added delete user Data method to utils package
</commit_message>
<xml_diff>
--- a/test_data/TestData.xlsx
+++ b/test_data/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\Documents\Python_Workspace\PM_SNM_Project\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\Documents\Python_Workspace\PM_SNM_Automation\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD11174-5C7A-477B-8FE5-82B6D769641E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE25385-1941-4974-BFB0-C2FD57319234}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -61,6 +61,13 @@
   </si>
   <si>
     <t>Arjuna@12345</t>
+  </si>
+  <si>
+    <t>test_create_user</t>
+  </si>
+  <si>
+    <t>TestUsr1,Mitel@123,Mitel@gmail.com,MitelFirst,MitelSecond,
+Business1,Business2,+917975935256,+918105855417</t>
   </si>
 </sst>
 </file>
@@ -104,9 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,16 +397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.90625" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -454,6 +464,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
After adding edit user emthod
</commit_message>
<xml_diff>
--- a/test_data/TestData.xlsx
+++ b/test_data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\Documents\Python_Workspace\PM_SNM_Automation\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE25385-1941-4974-BFB0-C2FD57319234}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E14ED2-29B2-4FC9-B753-3B9152B55945}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -68,6 +68,9 @@
   <si>
     <t>TestUsr1,Mitel@123,Mitel@gmail.com,MitelFirst,MitelSecond,
 Business1,Business2,+917975935256,+918105855417</t>
+  </si>
+  <si>
+    <t>test_edit_user</t>
   </si>
 </sst>
 </file>
@@ -397,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,6 +478,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added snm pom classes.
</commit_message>
<xml_diff>
--- a/test_data/TestData.xlsx
+++ b/test_data/TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\Documents\Python_Workspace\PM_SNM_Automation\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E14ED2-29B2-4FC9-B753-3B9152B55945}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00680E7-F86E-4BD5-9217-7E78B13B2592}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="1" r:id="rId1"/>
+    <sheet name="IP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -71,6 +72,12 @@
   </si>
   <si>
     <t>test_edit_user</t>
+  </si>
+  <si>
+    <t>http://10.211.162.111/wbm</t>
+  </si>
+  <si>
+    <t>http://10.211.162.111/mp</t>
   </si>
 </sst>
 </file>
@@ -402,7 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -493,4 +500,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E53A9E-ACD5-46DD-9427-7F06AD780F15}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added execute command utility method
</commit_message>
<xml_diff>
--- a/test_data/TestData.xlsx
+++ b/test_data/TestData.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\Documents\Python_Workspace\PM_SNM_Automation\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00680E7-F86E-4BD5-9217-7E78B13B2592}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACE0072-4DBE-4BA7-8FC2-042D87D0849E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="1" r:id="rId1"/>
-    <sheet name="IP" sheetId="2" r:id="rId2"/>
+    <sheet name="PMTestData" sheetId="3" r:id="rId2"/>
+    <sheet name="SNMTestData" sheetId="4" r:id="rId3"/>
+    <sheet name="IP" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -407,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,28 +476,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -503,10 +483,158 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECD1104-8824-4B0E-911A-8B0EFA495306}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.90625" customWidth="1"/>
+    <col min="2" max="2" width="41.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DB728E-D6A2-4728-8CDB-693BFA2A04D3}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.90625" customWidth="1"/>
+    <col min="2" max="2" width="41.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E53A9E-ACD5-46DD-9427-7F06AD780F15}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added snm method to execute commands in SNM.
</commit_message>
<xml_diff>
--- a/test_data/TestData.xlsx
+++ b/test_data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\Documents\Python_Workspace\PM_SNM_Automation\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACE0072-4DBE-4BA7-8FC2-042D87D0849E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38806B6-029D-4BB9-875B-1C2164F3904E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -80,6 +80,45 @@
   </si>
   <si>
     <t>http://10.211.162.111/mp</t>
+  </si>
+  <si>
+    <t>test_assign_extension_to_user</t>
+  </si>
+  <si>
+    <t>test_snm_valid_login</t>
+  </si>
+  <si>
+    <t>test_snmlogin_with_only_pwd</t>
+  </si>
+  <si>
+    <t>test_snm_invalidPWD_login</t>
+  </si>
+  <si>
+    <t>test_snm_invalidUserID_login</t>
+  </si>
+  <si>
+    <t>mxone_admin,Mxone@456</t>
+  </si>
+  <si>
+    <t>Mxone@456</t>
+  </si>
+  <si>
+    <t>mxone_admin,Mxone@999</t>
+  </si>
+  <si>
+    <t>mxone_budmin,Mxone@456</t>
+  </si>
+  <si>
+    <t>number_initiate -number 77777 -numbertype ex,
+extension -i -d 77777 -l 1 --csp 0,
+ip_extension -i -d 77777,
+TestUser2,
+Mitel@123,
+Mitel@gmail.com,
+77777,
+ip_extension -e -d 77777,
+extension -e -d 77777,
+number_end -number 77777..88888 -numbertype ex</t>
   </si>
 </sst>
 </file>
@@ -409,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,6 +515,50 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -484,10 +567,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECD1104-8824-4B0E-911A-8B0EFA495306}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.90625" customWidth="1"/>
+    <col min="2" max="2" width="60.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DB728E-D6A2-4728-8CDB-693BFA2A04D3}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,135 +653,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DB728E-D6A2-4728-8CDB-693BFA2A04D3}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="32.90625" customWidth="1"/>
-    <col min="2" max="2" width="41.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E53A9E-ACD5-46DD-9427-7F06AD780F15}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>